<commit_message>
actions and more other
</commit_message>
<xml_diff>
--- a/start_db.xlsx
+++ b/start_db.xlsx
@@ -8,30 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snckmykek\PycharmProjects\game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635B8ADC-15A8-4EAF-AADD-B400654C56A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD1078D-6595-41B9-8B7C-38515EF05F78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="975" windowWidth="19440" windowHeight="15000" tabRatio="927" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="975" windowWidth="19440" windowHeight="15000" tabRatio="927" firstSheet="16" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="15" r:id="rId1"/>
-    <sheet name="global_bonuses" sheetId="1" r:id="rId2"/>
-    <sheet name="manuscripts" sheetId="2" r:id="rId3"/>
-    <sheet name="manuscripts_lang" sheetId="3" r:id="rId4"/>
-    <sheet name="for_up_lvl" sheetId="4" r:id="rId5"/>
-    <sheet name="skills" sheetId="5" r:id="rId6"/>
-    <sheet name="skills_lang" sheetId="6" r:id="rId7"/>
-    <sheet name="chests" sheetId="7" r:id="rId8"/>
-    <sheet name="chests_lang" sheetId="8" r:id="rId9"/>
-    <sheet name="lvl_settings" sheetId="9" r:id="rId10"/>
-    <sheet name="lvl_settings_lang" sheetId="10" r:id="rId11"/>
-    <sheet name="levels" sheetId="11" r:id="rId12"/>
-    <sheet name="speech_and_descriptions" sheetId="12" r:id="rId13"/>
-    <sheet name="items_and_resources" sheetId="13" r:id="rId14"/>
-    <sheet name="items_and_resources_lang" sheetId="14" r:id="rId15"/>
-    <sheet name="level_colors" sheetId="18" r:id="rId16"/>
-    <sheet name="colors" sheetId="16" r:id="rId17"/>
-    <sheet name="game_bonuses" sheetId="17" r:id="rId18"/>
-    <sheet name="actions" sheetId="19" r:id="rId19"/>
+    <sheet name="game_settings" sheetId="25" r:id="rId2"/>
+    <sheet name="game_settings_lang" sheetId="26" r:id="rId3"/>
+    <sheet name="languages" sheetId="24" r:id="rId4"/>
+    <sheet name="global_bonuses" sheetId="1" r:id="rId5"/>
+    <sheet name="manuscripts" sheetId="2" r:id="rId6"/>
+    <sheet name="manuscripts_lang" sheetId="3" r:id="rId7"/>
+    <sheet name="for_up_lvl" sheetId="4" r:id="rId8"/>
+    <sheet name="skills" sheetId="5" r:id="rId9"/>
+    <sheet name="skills_lang" sheetId="6" r:id="rId10"/>
+    <sheet name="chests" sheetId="7" r:id="rId11"/>
+    <sheet name="chests_lang" sheetId="8" r:id="rId12"/>
+    <sheet name="lvl_settings" sheetId="9" r:id="rId13"/>
+    <sheet name="lvl_settings_lang" sheetId="10" r:id="rId14"/>
+    <sheet name="levels" sheetId="11" r:id="rId15"/>
+    <sheet name="speech_and_descriptions" sheetId="12" r:id="rId16"/>
+    <sheet name="items_and_resources" sheetId="13" r:id="rId17"/>
+    <sheet name="items_and_resources_lang" sheetId="14" r:id="rId18"/>
+    <sheet name="level_colors" sheetId="18" r:id="rId19"/>
+    <sheet name="colors" sheetId="16" r:id="rId20"/>
+    <sheet name="game_bonuses" sheetId="17" r:id="rId21"/>
+    <sheet name="actions" sheetId="19" r:id="rId22"/>
+    <sheet name="speech" sheetId="20" r:id="rId23"/>
+    <sheet name="miniatures" sheetId="23" r:id="rId24"/>
+    <sheet name="heroes" sheetId="22" r:id="rId25"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -43,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="257">
   <si>
     <t>bonus</t>
   </si>
@@ -631,6 +637,189 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>speech_order</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>speaker</t>
+  </si>
+  <si>
+    <t>hero</t>
+  </si>
+  <si>
+    <t>anti_hero</t>
+  </si>
+  <si>
+    <t>companion</t>
+  </si>
+  <si>
+    <t>Это тест для настройки комфортной скорости чтения.</t>
+  </si>
+  <si>
+    <t>Двигайте ползунок, чтобы изменить скорость появления текста.</t>
+  </si>
+  <si>
+    <t>К слову, у нас много других настроек для комфортной игры.</t>
+  </si>
+  <si>
+    <t>Настройки открываются из главного меню. Приятной игры!</t>
+  </si>
+  <si>
+    <t>dialog</t>
+  </si>
+  <si>
+    <t>This is a test for setting a comfortable reading speed.</t>
+  </si>
+  <si>
+    <t>Move the slider to change the speed at which text appears.</t>
+  </si>
+  <si>
+    <t>Вы всегда можете изменить скорость появления текста в настройках.</t>
+  </si>
+  <si>
+    <t>You can always change the speed of appearance of the text in the settings.</t>
+  </si>
+  <si>
+    <t>By the way, we have many other settings for a comfortable game.</t>
+  </si>
+  <si>
+    <t>Settings open from the main menu. Have a nice game!</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>after</t>
+  </si>
+  <si>
+    <t>current_loc_id</t>
+  </si>
+  <si>
+    <t>current_lvl_id</t>
+  </si>
+  <si>
+    <t>when_to_call</t>
+  </si>
+  <si>
+    <t>Кликните по экрану в область диалога, чтобы мгновенно увидеть всю реплику целиком. Попробуйте прямо сейчас, пока я буду писать этот очень длинный текст. \nПрирода Крайнего Севера разнообразна. Это ледники и каменистые пустыни Арктики, дрейфующие льды арктических морей, полоса тундр — то унылых, низменных и заболоченных, то сухих, покрытых летом пестрым ковром цветущих трав. Есть здесь заросли кустарников и одиночные деревья, рощицы лиственниц, елей, корявых, изогнутых берез. Крайний Север — это вереницы озер, густая сеть ручьев и рек, это морские побережья, то крутые, сглаженные волнами громады скал, то бесконечные пляжи с завалами плавника.</t>
+  </si>
+  <si>
+    <t>Click on the screen in the dialog area to instantly see the entire replica. Try it now while I am writing this very long text. \nThe nature of the Far North is diverse. These are glaciers and stony deserts of the Arctic, drifting ice of the Arctic seas, a strip of tundra - then dull, low-lying and marshy, then dry, flowering grasses covered with a colorful carpet in summer. There are bushes and solitary trees, groves of larch, spruce, clumsy, curved birches. The Far North is a series of lakes, a dense network of streams and rivers, these are sea coasts, then steep, smooth waves of rocks smoothed by waves, then endless beaches with fin blockages.</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>Hero</t>
+  </si>
+  <si>
+    <t>Companion</t>
+  </si>
+  <si>
+    <t>Antihero</t>
+  </si>
+  <si>
+    <t>images/heroes/hero.png</t>
+  </si>
+  <si>
+    <t>images/heroes/companion.png</t>
+  </si>
+  <si>
+    <t>images/heroes/anti_hero.png</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>Тест 1</t>
+  </si>
+  <si>
+    <t>Тест 2</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>miniature_order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тестируем тестовый тест тестируем тестовый тест. Тестируем тестовый тест тестируем тестовый тест. Тестируем тестовый тест тестируем тестовый тест. </t>
+  </si>
+  <si>
+    <t>images/miniatures/farewell_note.png</t>
+  </si>
+  <si>
+    <t>miniature</t>
+  </si>
+  <si>
+    <t>images/miniatures/fon2.png</t>
+  </si>
+  <si>
+    <t>images/miniatures/world_map_2.png</t>
+  </si>
+  <si>
+    <t>Ghbdtn</t>
+  </si>
+  <si>
+    <t>images/miniatures/Screenshot_4.png</t>
+  </si>
+  <si>
+    <t>Апаснасть это ага да, а вот не апасность это нет и нет проблема да.</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>setting</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>SPEECH_SPEED</t>
+  </si>
+  <si>
+    <t>MUSIC_VOLUME</t>
+  </si>
+  <si>
+    <t>Язык</t>
+  </si>
+  <si>
+    <t>Скорость реплик</t>
+  </si>
+  <si>
+    <t>Громкость музыки</t>
+  </si>
+  <si>
+    <t>CUBE_MOVE_VOLUME</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Speech speed</t>
+  </si>
+  <si>
+    <t>Music volume</t>
+  </si>
+  <si>
+    <t>Volume of movement of field elements</t>
+  </si>
+  <si>
+    <t>Громкость движения элементов поля</t>
   </si>
 </sst>
 </file>
@@ -672,8 +861,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -954,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5054111A-95ED-49E4-8765-DCCFD7FF7C9E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,12 +1181,1326 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AD491E-238D-40A0-BF69-62DA4910C578}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAD34FE-FDAD-4091-B3A7-8C7652685EE9}">
+  <dimension ref="A1:F49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>120</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30">
+        <v>12</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31">
+        <v>13</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32">
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33">
+        <v>15</v>
+      </c>
+      <c r="E33">
+        <v>500</v>
+      </c>
+      <c r="F33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>18</v>
+      </c>
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43">
+        <v>9</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>18</v>
+      </c>
+      <c r="B45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45">
+        <v>11</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46">
+        <v>12</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>18</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47">
+        <v>13</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48">
+        <v>14</v>
+      </c>
+      <c r="E48">
+        <v>50</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>18</v>
+      </c>
+      <c r="B49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49">
+        <v>15</v>
+      </c>
+      <c r="E49">
+        <v>1000</v>
+      </c>
+      <c r="F49">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70441C2-9BE7-4A77-92B1-06BD72BFF458}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD84CBF2-2FCD-4BAB-9F12-9D608941CFC1}">
   <dimension ref="A1:N40"/>
   <sheetViews>
@@ -2546,7 +4052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C736FF81-475B-44CB-BBE7-85AE4FF4518E}">
   <dimension ref="A1:D79"/>
   <sheetViews>
@@ -3671,7 +5177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF433431-3E27-4F68-AE1D-CEA2AAC4AC33}">
   <dimension ref="A1:G118"/>
   <sheetViews>
@@ -6404,7 +7910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D0448D-EAA4-4309-A09D-781E5BD205BB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -6444,11 +7950,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16AB8FE-0428-45A1-8AB6-FCC19B6524B4}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -7009,7 +8515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C990E5FE-8494-461C-B6B6-EB9EDED6294D}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -7574,7 +9080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC213907-93D9-459A-BA5D-3C4A0E992FFA}">
   <dimension ref="A1:C58"/>
   <sheetViews>
@@ -8227,7 +9733,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E6919C-E057-4D2B-B68A-4F60A7DC347A}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="A5:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37B25C5-20E3-4F0D-8BBE-E6A10F75F981}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -8395,7 +9959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F0E707-D929-4B6C-A217-6304DEAD0A83}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -8601,22 +10165,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A4338D-0251-443F-8906-A26B275FB1A2}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>191</v>
       </c>
@@ -8633,10 +10198,13 @@
         <v>30</v>
       </c>
       <c r="F1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -8652,11 +10220,14 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8672,11 +10243,14 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -8692,11 +10266,14 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -8712,11 +10289,14 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -8732,11 +10312,14 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>214</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -8752,7 +10335,125 @@
       <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>229</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>229</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>229</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>237</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>213</v>
+      </c>
+      <c r="G12">
         <v>0</v>
       </c>
     </row>
@@ -8762,7 +10463,747 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA7D8AE-63E0-4282-8FD1-27B1D30F5777}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="60.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" t="s">
+        <v>221</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" t="s">
+        <v>221</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14" t="s">
+        <v>222</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D16" t="s">
+        <v>221</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" t="s">
+        <v>222</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264761C5-4E4D-4D79-9F3D-95D17886862B}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="49" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>241</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C19161-88A0-48F0-AB89-48D18599DE1F}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD388A19-DA49-47C3-9BA2-9B098AC55C3D}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5507FEC-0EAE-4F31-A744-6B3BBD5949E4}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -8849,7 +11290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD188B1-CEFB-4274-B0D8-746CFAD72EEC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -8964,7 +11405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF79BA3-B18F-4EBC-8518-A80D55AF2F98}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -9059,7 +11500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDA5321-EF7D-4709-8664-0533BE6CC5BF}">
   <dimension ref="A1:D441"/>
   <sheetViews>
@@ -15254,7 +17695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8924E574-FD9E-4C2E-B8D8-F98B6EC90312}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -15433,1302 +17874,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AD491E-238D-40A0-BF69-62DA4910C578}">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>194</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" t="s">
-        <v>195</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>195</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>195</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAD34FE-FDAD-4091-B3A7-8C7652685EE9}">
-  <dimension ref="A1:F49"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13">
-        <v>11</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14">
-        <v>12</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15">
-        <v>13</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16">
-        <v>14</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17">
-        <v>15</v>
-      </c>
-      <c r="E17">
-        <v>120</v>
-      </c>
-      <c r="F17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>17</v>
-      </c>
-      <c r="B22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22">
-        <v>4</v>
-      </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>17</v>
-      </c>
-      <c r="B23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23">
-        <v>5</v>
-      </c>
-      <c r="E23">
-        <v>3</v>
-      </c>
-      <c r="F23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-      <c r="E24">
-        <v>3</v>
-      </c>
-      <c r="F24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>17</v>
-      </c>
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25">
-        <v>7</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
-      </c>
-      <c r="F25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>17</v>
-      </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26">
-        <v>8</v>
-      </c>
-      <c r="E26">
-        <v>3</v>
-      </c>
-      <c r="F26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>17</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27">
-        <v>9</v>
-      </c>
-      <c r="E27">
-        <v>3</v>
-      </c>
-      <c r="F27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>17</v>
-      </c>
-      <c r="B28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28">
-        <v>10</v>
-      </c>
-      <c r="E28">
-        <v>3</v>
-      </c>
-      <c r="F28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>17</v>
-      </c>
-      <c r="B29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29">
-        <v>11</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>17</v>
-      </c>
-      <c r="B30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30">
-        <v>12</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="F30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>17</v>
-      </c>
-      <c r="B31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31">
-        <v>13</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-      <c r="F31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>17</v>
-      </c>
-      <c r="B32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32">
-        <v>14</v>
-      </c>
-      <c r="E32">
-        <v>30</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>17</v>
-      </c>
-      <c r="B33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33">
-        <v>15</v>
-      </c>
-      <c r="E33">
-        <v>500</v>
-      </c>
-      <c r="F33">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>18</v>
-      </c>
-      <c r="B34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>5</v>
-      </c>
-      <c r="F34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>18</v>
-      </c>
-      <c r="B35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>5</v>
-      </c>
-      <c r="F35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>18</v>
-      </c>
-      <c r="B36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-      <c r="E36">
-        <v>5</v>
-      </c>
-      <c r="F36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>18</v>
-      </c>
-      <c r="B37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37">
-        <v>3</v>
-      </c>
-      <c r="E37">
-        <v>5</v>
-      </c>
-      <c r="F37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>18</v>
-      </c>
-      <c r="B38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38">
-        <v>4</v>
-      </c>
-      <c r="E38">
-        <v>5</v>
-      </c>
-      <c r="F38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>18</v>
-      </c>
-      <c r="B39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39">
-        <v>5</v>
-      </c>
-      <c r="E39">
-        <v>5</v>
-      </c>
-      <c r="F39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>18</v>
-      </c>
-      <c r="B40" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40">
-        <v>6</v>
-      </c>
-      <c r="E40">
-        <v>5</v>
-      </c>
-      <c r="F40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>18</v>
-      </c>
-      <c r="B41" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41">
-        <v>7</v>
-      </c>
-      <c r="E41">
-        <v>5</v>
-      </c>
-      <c r="F41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>18</v>
-      </c>
-      <c r="B42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42">
-        <v>8</v>
-      </c>
-      <c r="E42">
-        <v>5</v>
-      </c>
-      <c r="F42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>18</v>
-      </c>
-      <c r="B43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43">
-        <v>9</v>
-      </c>
-      <c r="E43">
-        <v>5</v>
-      </c>
-      <c r="F43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>18</v>
-      </c>
-      <c r="B44" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" t="s">
-        <v>69</v>
-      </c>
-      <c r="D44">
-        <v>10</v>
-      </c>
-      <c r="E44">
-        <v>5</v>
-      </c>
-      <c r="F44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>18</v>
-      </c>
-      <c r="B45" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45">
-        <v>11</v>
-      </c>
-      <c r="E45">
-        <v>3</v>
-      </c>
-      <c r="F45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>18</v>
-      </c>
-      <c r="B46" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46">
-        <v>12</v>
-      </c>
-      <c r="E46">
-        <v>3</v>
-      </c>
-      <c r="F46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>18</v>
-      </c>
-      <c r="B47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47">
-        <v>13</v>
-      </c>
-      <c r="E47">
-        <v>3</v>
-      </c>
-      <c r="F47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>18</v>
-      </c>
-      <c r="B48" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" t="s">
-        <v>69</v>
-      </c>
-      <c r="D48">
-        <v>14</v>
-      </c>
-      <c r="E48">
-        <v>50</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>18</v>
-      </c>
-      <c r="B49" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49">
-        <v>15</v>
-      </c>
-      <c r="E49">
-        <v>1000</v>
-      </c>
-      <c r="F49">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70441C2-9BE7-4A77-92B1-06BD72BFF458}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>